<commit_message>
simulazione partendo da risultati europee
</commit_message>
<xml_diff>
--- a/dati/corrispondenza_liste.xlsx
+++ b/dati/corrispondenza_liste.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Repos\elezioni-EMR\dati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{507610AE-CDE7-40E6-848F-DE71B2596AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51C9E496-A430-40DF-A8A3-4F3137E0748A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-19320" yWindow="-120" windowWidth="19440" windowHeight="14880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="64">
   <si>
     <t>ELEZIONE</t>
   </si>
@@ -210,9 +210,6 @@
   </si>
   <si>
     <t>LISTA_ORIGINALE</t>
-  </si>
-  <si>
-    <t>AVS</t>
   </si>
   <si>
     <t>STATI UNITI D'EUROPA</t>
@@ -1075,8 +1072,8 @@
   <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I1" sqref="I1"/>
+      <pane ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1084,7 @@
     <col min="15" max="15" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="123" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="137.25" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -1095,7 +1092,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -1104,7 +1101,7 @@
         <v>13</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>57</v>
@@ -1119,13 +1116,13 @@
         <v>12</v>
       </c>
       <c r="K1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>63</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>5</v>
@@ -1136,10 +1133,10 @@
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -1150,7 +1147,7 @@
         <v>57</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G3">
         <v>1</v>
@@ -1158,10 +1155,10 @@
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="K4">
         <v>1</v>
@@ -1169,10 +1166,10 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L5">
         <v>1</v>
@@ -1180,10 +1177,10 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B6" t="s">
         <v>63</v>
-      </c>
-      <c r="B6" t="s">
-        <v>64</v>
       </c>
       <c r="C6">
         <v>1</v>

</xml_diff>

<commit_message>
Lista De Pascale, nuovi grafici
</commit_message>
<xml_diff>
--- a/dati/corrispondenza_liste.xlsx
+++ b/dati/corrispondenza_liste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Repos\elezioni-EMR\dati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C1E9926-A9E0-46E8-A43F-A4ED33B99612}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0478F632-C073-447B-8680-4C36533CB720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="66">
   <si>
     <t>ELEZIONE</t>
   </si>
@@ -225,6 +225,12 @@
   </si>
   <si>
     <t>europee2024</t>
+  </si>
+  <si>
+    <t>DE PASCALE</t>
+  </si>
+  <si>
+    <t>ALLEANZA VERDI SINISTRA</t>
   </si>
 </sst>
 </file>
@@ -1069,22 +1075,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O58"/>
+  <dimension ref="A1:P58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A29" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E50" sqref="E50"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.42578125" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="14" width="4.85546875" customWidth="1"/>
-    <col min="15" max="15" width="5.28515625" customWidth="1"/>
+    <col min="3" max="15" width="4.85546875" customWidth="1"/>
+    <col min="16" max="16" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="137.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" ht="129" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -1092,104 +1098,104 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>49</v>
+        <v>65</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
       <c r="B2" t="s">
         <v>63</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
       </c>
-      <c r="K4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="L5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>62</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="M6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1200,51 +1206,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="I8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
-      <c r="J9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
-      <c r="N10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="O10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="K11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1255,186 +1261,186 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="O13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
-      <c r="H14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
-      <c r="L15">
-        <v>0.5</v>
-      </c>
       <c r="M15">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N15">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="O16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="J17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
       <c r="B19" t="s">
         <v>1</v>
       </c>
-      <c r="E19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
       </c>
-      <c r="M21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="J22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>
       </c>
-      <c r="K23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
       </c>
-      <c r="O24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
-      <c r="K25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
       <c r="B26" t="s">
         <v>18</v>
       </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
       <c r="B27" t="s">
         <v>18</v>
       </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
       <c r="B28" t="s">
         <v>18</v>
       </c>
-      <c r="D28">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -1445,57 +1451,57 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
       </c>
-      <c r="I30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
       <c r="B31" t="s">
         <v>18</v>
       </c>
-      <c r="I31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
       <c r="B32" t="s">
         <v>18</v>
       </c>
-      <c r="L32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
       <c r="B33" t="s">
         <v>18</v>
       </c>
-      <c r="H33">
-        <v>0.33</v>
-      </c>
       <c r="I33">
         <v>0.33</v>
       </c>
       <c r="J33">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K33">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1506,40 +1512,40 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
       <c r="B35" t="s">
         <v>29</v>
       </c>
-      <c r="J35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
       <c r="B36" t="s">
         <v>29</v>
       </c>
-      <c r="H36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B37" t="s">
         <v>29</v>
       </c>
-      <c r="F37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1547,16 +1553,16 @@
         <v>29</v>
       </c>
       <c r="C38">
-        <v>0.33</v>
+        <v>0.3</v>
       </c>
       <c r="D38">
         <v>0.33</v>
       </c>
-      <c r="M38">
+      <c r="N38">
         <v>0.33</v>
       </c>
     </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1570,162 +1576,162 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
       <c r="B40" t="s">
         <v>29</v>
       </c>
-      <c r="M40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="N40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
       <c r="B41" t="s">
         <v>29</v>
       </c>
-      <c r="J41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
       <c r="B42" t="s">
         <v>29</v>
       </c>
-      <c r="O42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
       <c r="B43" t="s">
         <v>29</v>
       </c>
-      <c r="K43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
       <c r="B44" t="s">
         <v>29</v>
       </c>
-      <c r="L44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
       <c r="B45" t="s">
         <v>40</v>
       </c>
-      <c r="K45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>41</v>
       </c>
       <c r="B46" t="s">
         <v>40</v>
       </c>
-      <c r="L46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>42</v>
       </c>
       <c r="B47" t="s">
         <v>40</v>
       </c>
-      <c r="H47">
-        <v>0.33</v>
-      </c>
       <c r="I47">
         <v>0.33</v>
       </c>
       <c r="J47">
         <v>0.33</v>
       </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="K47">
+        <v>0.33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>43</v>
       </c>
       <c r="B48" t="s">
         <v>40</v>
       </c>
-      <c r="F48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="G48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>44</v>
       </c>
       <c r="B49" t="s">
         <v>40</v>
       </c>
-      <c r="L49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="M49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>45</v>
       </c>
       <c r="B50" t="s">
         <v>40</v>
       </c>
-      <c r="F50">
-        <v>0.5</v>
-      </c>
       <c r="G50">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="H50">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>46</v>
       </c>
       <c r="B51" t="s">
         <v>40</v>
       </c>
-      <c r="I51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="J51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>47</v>
       </c>
       <c r="B52" t="s">
         <v>40</v>
       </c>
-      <c r="G52">
-        <v>0.5</v>
-      </c>
       <c r="H52">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="I52">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -1736,7 +1742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -1747,47 +1753,47 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>50</v>
       </c>
       <c r="B55" t="s">
         <v>40</v>
       </c>
-      <c r="E55">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F55">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>51</v>
       </c>
       <c r="B56" t="s">
         <v>40</v>
       </c>
-      <c r="E56">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="F56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>52</v>
       </c>
       <c r="B57" t="s">
         <v>40</v>
       </c>
-      <c r="K57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="L57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>53</v>
       </c>
       <c r="B58" t="s">
         <v>29</v>
       </c>
-      <c r="O58">
+      <c r="P58">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
sondaggi + ipotesi Nicola
</commit_message>
<xml_diff>
--- a/dati/corrispondenza_liste.xlsx
+++ b/dati/corrispondenza_liste.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Luca\Repos\elezioni-EMR\dati\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0478F632-C073-447B-8680-4C36533CB720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1FAF11-0833-4050-961D-99F6F733EB61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="67">
   <si>
     <t>ELEZIONE</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>ALLEANZA VERDI SINISTRA</t>
+  </si>
+  <si>
+    <t>CENTRO</t>
   </si>
 </sst>
 </file>
@@ -1075,22 +1078,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P58"/>
+  <dimension ref="A1:O58"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="47.42578125" customWidth="1"/>
     <col min="2" max="2" width="20.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="15" width="4.85546875" customWidth="1"/>
-    <col min="16" max="16" width="5.28515625" customWidth="1"/>
+    <col min="3" max="14" width="4.85546875" customWidth="1"/>
+    <col min="15" max="15" width="5.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="129" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" ht="129" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>58</v>
       </c>
@@ -1110,37 +1113,34 @@
         <v>13</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>59</v>
+        <v>66</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>12</v>
+        <v>60</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>62</v>
+        <v>5</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="P1" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>59</v>
       </c>
@@ -1151,51 +1151,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>57</v>
       </c>
       <c r="B3" t="s">
         <v>63</v>
       </c>
-      <c r="H3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
       <c r="B4" t="s">
         <v>63</v>
       </c>
-      <c r="L4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>61</v>
       </c>
       <c r="B5" t="s">
         <v>63</v>
       </c>
-      <c r="M5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>62</v>
       </c>
       <c r="B6" t="s">
         <v>63</v>
       </c>
-      <c r="N6">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -1206,51 +1206,51 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
       <c r="B8" t="s">
         <v>1</v>
       </c>
-      <c r="J8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
       </c>
-      <c r="K9">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
         <v>1</v>
       </c>
-      <c r="O10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="N10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
         <v>1</v>
       </c>
-      <c r="L11">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -1261,65 +1261,65 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
       <c r="B13" t="s">
         <v>1</v>
       </c>
-      <c r="P13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
       <c r="B14" t="s">
         <v>1</v>
       </c>
-      <c r="I14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
       </c>
+      <c r="L15">
+        <v>0.5</v>
+      </c>
       <c r="M15">
         <v>0.5</v>
       </c>
-      <c r="N15">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
       <c r="B16" t="s">
         <v>1</v>
       </c>
-      <c r="P16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
       <c r="B17" t="s">
         <v>1</v>
       </c>
-      <c r="K17">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
         <v>54</v>
       </c>
@@ -1330,7 +1330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1341,73 +1341,73 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>1</v>
       </c>
-      <c r="P20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>15</v>
       </c>
       <c r="B21" t="s">
         <v>1</v>
       </c>
-      <c r="N21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>16</v>
       </c>
       <c r="B22" t="s">
         <v>1</v>
       </c>
-      <c r="K22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>17</v>
       </c>
       <c r="B23" t="s">
         <v>18</v>
       </c>
-      <c r="L23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>19</v>
       </c>
       <c r="B24" t="s">
         <v>18</v>
       </c>
-      <c r="P24">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>20</v>
       </c>
       <c r="B25" t="s">
         <v>18</v>
       </c>
-      <c r="L25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>21</v>
       </c>
@@ -1418,7 +1418,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
         <v>55</v>
       </c>
@@ -1429,7 +1429,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>22</v>
       </c>
@@ -1440,7 +1440,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>23</v>
       </c>
@@ -1451,57 +1451,57 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>24</v>
       </c>
       <c r="B30" t="s">
         <v>18</v>
       </c>
-      <c r="J30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>25</v>
       </c>
       <c r="B31" t="s">
         <v>18</v>
       </c>
-      <c r="J31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>26</v>
       </c>
       <c r="B32" t="s">
         <v>18</v>
       </c>
-      <c r="M32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>27</v>
       </c>
       <c r="B33" t="s">
         <v>18</v>
       </c>
+      <c r="H33">
+        <v>0.33</v>
+      </c>
       <c r="I33">
         <v>0.33</v>
       </c>
       <c r="J33">
         <v>0.33</v>
       </c>
-      <c r="K33">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>28</v>
       </c>
@@ -1512,29 +1512,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>30</v>
       </c>
       <c r="B35" t="s">
         <v>29</v>
       </c>
-      <c r="K35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>31</v>
       </c>
       <c r="B36" t="s">
         <v>29</v>
       </c>
-      <c r="I36">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="H36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
         <v>56</v>
       </c>
@@ -1545,7 +1545,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>32</v>
       </c>
@@ -1558,11 +1558,11 @@
       <c r="D38">
         <v>0.33</v>
       </c>
-      <c r="N38">
+      <c r="M38">
         <v>0.33</v>
       </c>
     </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>33</v>
       </c>
@@ -1576,101 +1576,101 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>34</v>
       </c>
       <c r="B40" t="s">
         <v>29</v>
       </c>
-      <c r="N40">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="M40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>35</v>
       </c>
       <c r="B41" t="s">
         <v>29</v>
       </c>
-      <c r="K41">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>36</v>
       </c>
       <c r="B42" t="s">
         <v>29</v>
       </c>
-      <c r="P42">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>37</v>
       </c>
       <c r="B43" t="s">
         <v>29</v>
       </c>
-      <c r="L43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>38</v>
       </c>
       <c r="B44" t="s">
         <v>29</v>
       </c>
-      <c r="M44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>39</v>
       </c>
       <c r="B45" t="s">
         <v>40</v>
       </c>
-      <c r="L45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>41</v>
       </c>
       <c r="B46" t="s">
         <v>40</v>
       </c>
-      <c r="M46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>42</v>
       </c>
       <c r="B47" t="s">
         <v>40</v>
       </c>
+      <c r="H47">
+        <v>0.33</v>
+      </c>
       <c r="I47">
         <v>0.33</v>
       </c>
       <c r="J47">
         <v>0.33</v>
       </c>
-      <c r="K47">
-        <v>0.33</v>
-      </c>
-    </row>
-    <row r="48" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>43</v>
       </c>
@@ -1681,18 +1681,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>44</v>
       </c>
       <c r="B49" t="s">
         <v>40</v>
       </c>
-      <c r="M49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="L49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>45</v>
       </c>
@@ -1700,38 +1700,35 @@
         <v>40</v>
       </c>
       <c r="G50">
-        <v>0.5</v>
-      </c>
-      <c r="H50">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>46</v>
       </c>
       <c r="B51" t="s">
         <v>40</v>
       </c>
-      <c r="J51">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="I51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>47</v>
       </c>
       <c r="B52" t="s">
         <v>40</v>
       </c>
+      <c r="G52">
+        <v>0.5</v>
+      </c>
       <c r="H52">
         <v>0.5</v>
       </c>
-      <c r="I52">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>48</v>
       </c>
@@ -1742,7 +1739,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>49</v>
       </c>
@@ -1753,7 +1750,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>50</v>
       </c>
@@ -1764,7 +1761,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>51</v>
       </c>
@@ -1775,25 +1772,25 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>52</v>
       </c>
       <c r="B57" t="s">
         <v>40</v>
       </c>
-      <c r="L57">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="K57">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>53</v>
       </c>
       <c r="B58" t="s">
         <v>29</v>
       </c>
-      <c r="P58">
+      <c r="O58">
         <v>1</v>
       </c>
     </row>

</xml_diff>